<commit_message>
login test cases added
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\eclipse-workspace\OpenCart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132C27A9-852A-4844-9D61-EB89A899AC6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E2C39C-EC23-47E7-8F4E-C0387D649A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -42,15 +42,9 @@
     <t>password</t>
   </si>
   <si>
-    <t>res</t>
-  </si>
-  <si>
     <t>lakshmi@yahoo.com</t>
   </si>
   <si>
-    <t>Lakshmi</t>
-  </si>
-  <si>
     <t>Valid</t>
   </si>
   <si>
@@ -63,26 +57,35 @@
     <t>Invalid</t>
   </si>
   <si>
-    <t>laks@yahoo.com</t>
-  </si>
-  <si>
     <t>xyz</t>
   </si>
   <si>
-    <t>pavanoltraining@gmail.com</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
     <t>topcoders1@gmail.com</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>expected_result</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>account_login_validation</t>
+  </si>
+  <si>
+    <t>account_login_browser_back</t>
+  </si>
+  <si>
+    <t>account_login_logout_browser_back</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +101,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +117,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -141,20 +150,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -470,95 +474,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FCF78-0A3E-40BF-9E26-11C478AF56E2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1234</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1234</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="C7" s="2">
+        <v>1234</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4">
+      <c r="C8" s="2">
         <v>1234</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D3BE7519-95C3-4ACD-9AB4-5385C9508082}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{968262D0-AE14-41EF-AB8A-08B3F886E797}"/>
-    <hyperlink ref="B6" r:id="rId6" display="test@123" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
+    <hyperlink ref="C2" r:id="rId3" display="test@123" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
+    <hyperlink ref="C7" r:id="rId4" display="test@123" xr:uid="{1B167569-FED0-4E6B-9339-C77B7F48AA3B}"/>
+    <hyperlink ref="C8" r:id="rId5" display="test@123" xr:uid="{8A955895-14A5-4458-B3CA-1527B3113BB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
login test cases completed
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\eclipse-workspace\OpenCart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E2C39C-EC23-47E7-8F4E-C0387D649A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16850C6-6C40-4734-8E6C-D47923930060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
-  <si>
-    <t>username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>password</t>
   </si>
@@ -79,6 +76,21 @@
   </si>
   <si>
     <t>account_login_logout_browser_back</t>
+  </si>
+  <si>
+    <t>account_login_password_copy</t>
+  </si>
+  <si>
+    <t>copypassword</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>account_login_close_browser</t>
+  </si>
+  <si>
+    <t>account_login_navigating</t>
   </si>
 </sst>
 </file>
@@ -122,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -145,12 +157,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -159,6 +180,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -474,141 +498,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FCF78-0A3E-40BF-9E26-11C478AF56E2}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
         <v>1234</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
         <v>1234</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
         <v>1234</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2">
         <v>1234</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1234</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{8456409A-CACC-4B7E-B78E-75E713148E0E}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
-    <hyperlink ref="C2" r:id="rId3" display="test@123" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
-    <hyperlink ref="C7" r:id="rId4" display="test@123" xr:uid="{1B167569-FED0-4E6B-9339-C77B7F48AA3B}"/>
-    <hyperlink ref="C8" r:id="rId5" display="test@123" xr:uid="{8A955895-14A5-4458-B3CA-1527B3113BB2}"/>
+    <hyperlink ref="C11" r:id="rId1" display="test@123" xr:uid="{C7054731-23E0-4A84-8B5D-BB054B22B5A2}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{47B31D2A-C073-45C7-B5A1-5333717F1FC2}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{901C67FB-F0BE-43A1-9506-DD8177552BFB}"/>
+    <hyperlink ref="C2" r:id="rId4" display="test@123" xr:uid="{0971D0BC-7E3F-45F7-A27F-C37A4D9B4FCA}"/>
+    <hyperlink ref="C7" r:id="rId5" display="test@123" xr:uid="{5001AA88-2244-4BDC-AD76-7A5C2B4DB009}"/>
+    <hyperlink ref="C8" r:id="rId6" display="test@123" xr:uid="{759B6A73-7F9C-478F-A48D-F027481EACCD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>